<commit_message>
fixing restaurant price bug
</commit_message>
<xml_diff>
--- a/data/ml_perform_crossval_raw_2022-11-12.xlsx
+++ b/data/ml_perform_crossval_raw_2022-11-12.xlsx
@@ -483,10 +483,10 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>2.031429529190063</v>
+        <v>0.8657803535461426</v>
       </c>
       <c r="C2">
-        <v>0.09110140800476074</v>
+        <v>0.05122542381286621</v>
       </c>
       <c r="D2">
         <v>0.08248846559198129</v>
@@ -524,10 +524,10 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>2.097284317016602</v>
+        <v>0.7299034595489502</v>
       </c>
       <c r="C3">
-        <v>0.1318421363830566</v>
+        <v>0.02620148658752441</v>
       </c>
       <c r="D3">
         <v>0.08336360897600377</v>
@@ -565,10 +565,10 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>2.573634386062622</v>
+        <v>0.70076584815979</v>
       </c>
       <c r="C4">
-        <v>0.1316530704498291</v>
+        <v>0.02925825119018555</v>
       </c>
       <c r="D4">
         <v>0.07738908452151397</v>
@@ -606,10 +606,10 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>2.46354079246521</v>
+        <v>0.7345669269561768</v>
       </c>
       <c r="C5">
-        <v>0.1091322898864746</v>
+        <v>0.03012681007385254</v>
       </c>
       <c r="D5">
         <v>0.07642599360667264</v>
@@ -647,10 +647,10 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>1.492295742034912</v>
+        <v>0.8423118591308594</v>
       </c>
       <c r="C6">
-        <v>0.08769822120666504</v>
+        <v>0.04671835899353027</v>
       </c>
       <c r="D6">
         <v>0.07733484620799465</v>
@@ -688,10 +688,10 @@
         <v>0</v>
       </c>
       <c r="B7">
-        <v>0.51450514793396</v>
+        <v>0.2211968898773193</v>
       </c>
       <c r="C7">
-        <v>0.02293777465820312</v>
+        <v>0.007737874984741211</v>
       </c>
       <c r="D7">
         <v>0.07709498919182382</v>
@@ -729,10 +729,10 @@
         <v>1</v>
       </c>
       <c r="B8">
-        <v>0.5820577144622803</v>
+        <v>0.2312071323394775</v>
       </c>
       <c r="C8">
-        <v>0.006981611251831055</v>
+        <v>0.006039857864379883</v>
       </c>
       <c r="D8">
         <v>0.07848687519176649</v>
@@ -770,10 +770,10 @@
         <v>2</v>
       </c>
       <c r="B9">
-        <v>0.510711669921875</v>
+        <v>0.2614874839782715</v>
       </c>
       <c r="C9">
-        <v>0.01196098327636719</v>
+        <v>0.005982637405395508</v>
       </c>
       <c r="D9">
         <v>0.07388282132229627</v>
@@ -811,10 +811,10 @@
         <v>3</v>
       </c>
       <c r="B10">
-        <v>0.5259039402008057</v>
+        <v>0.2686727046966553</v>
       </c>
       <c r="C10">
-        <v>0.008684158325195312</v>
+        <v>0.004987239837646484</v>
       </c>
       <c r="D10">
         <v>0.07221064408067915</v>
@@ -852,10 +852,10 @@
         <v>4</v>
       </c>
       <c r="B11">
-        <v>0.5087299346923828</v>
+        <v>0.2399487495422363</v>
       </c>
       <c r="C11">
-        <v>0.007979631423950195</v>
+        <v>0.007350444793701172</v>
       </c>
       <c r="D11">
         <v>0.07362224466149696</v>
@@ -893,10 +893,10 @@
         <v>0</v>
       </c>
       <c r="B12">
-        <v>1.21628212928772</v>
+        <v>0.5863428115844727</v>
       </c>
       <c r="C12">
-        <v>0.1009278297424316</v>
+        <v>0.04588222503662109</v>
       </c>
       <c r="D12">
         <v>0.08497730553692706</v>
@@ -934,10 +934,10 @@
         <v>1</v>
       </c>
       <c r="B13">
-        <v>3.260987997055054</v>
+        <v>0.5235490798950195</v>
       </c>
       <c r="C13">
-        <v>0.09176445007324219</v>
+        <v>0.04365944862365723</v>
       </c>
       <c r="D13">
         <v>0.08657808696006813</v>
@@ -975,10 +975,10 @@
         <v>2</v>
       </c>
       <c r="B14">
-        <v>1.372373104095459</v>
+        <v>0.50528883934021</v>
       </c>
       <c r="C14">
-        <v>0.0978095531463623</v>
+        <v>0.04187989234924316</v>
       </c>
       <c r="D14">
         <v>0.07924330038193264</v>
@@ -1016,10 +1016,10 @@
         <v>3</v>
       </c>
       <c r="B15">
-        <v>1.371229410171509</v>
+        <v>0.5484380722045898</v>
       </c>
       <c r="C15">
-        <v>0.07579517364501953</v>
+        <v>0.04631161689758301</v>
       </c>
       <c r="D15">
         <v>0.07605982112904239</v>
@@ -1057,10 +1057,10 @@
         <v>4</v>
       </c>
       <c r="B16">
-        <v>2.012930870056152</v>
+        <v>0.603208065032959</v>
       </c>
       <c r="C16">
-        <v>0.0788114070892334</v>
+        <v>0.04237270355224609</v>
       </c>
       <c r="D16">
         <v>0.07344823173092267</v>
@@ -1098,10 +1098,10 @@
         <v>0</v>
       </c>
       <c r="B17">
-        <v>5.585836887359619</v>
+        <v>2.458347082138062</v>
       </c>
       <c r="C17">
-        <v>0.08280491828918457</v>
+        <v>0.05089139938354492</v>
       </c>
       <c r="D17">
         <v>0.08434027048990006</v>
@@ -1139,10 +1139,10 @@
         <v>1</v>
       </c>
       <c r="B18">
-        <v>4.430322408676147</v>
+        <v>2.406069993972778</v>
       </c>
       <c r="C18">
-        <v>0.06685781478881836</v>
+        <v>0.02800774574279785</v>
       </c>
       <c r="D18">
         <v>0.08478563673003976</v>
@@ -1180,10 +1180,10 @@
         <v>2</v>
       </c>
       <c r="B19">
-        <v>4.032682657241821</v>
+        <v>2.095066547393799</v>
       </c>
       <c r="C19">
-        <v>0.06810569763183594</v>
+        <v>0.02736568450927734</v>
       </c>
       <c r="D19">
         <v>0.07834314593365685</v>
@@ -1221,10 +1221,10 @@
         <v>3</v>
       </c>
       <c r="B20">
-        <v>3.990455150604248</v>
+        <v>2.166279792785645</v>
       </c>
       <c r="C20">
-        <v>0.05707263946533203</v>
+        <v>0.02931594848632812</v>
       </c>
       <c r="D20">
         <v>0.07840076552563764</v>
@@ -1262,10 +1262,10 @@
         <v>4</v>
       </c>
       <c r="B21">
-        <v>4.087456464767456</v>
+        <v>2.101835489273071</v>
       </c>
       <c r="C21">
-        <v>0.06685924530029297</v>
+        <v>0.02836465835571289</v>
       </c>
       <c r="D21">
         <v>0.07625208995775208</v>
@@ -1303,10 +1303,10 @@
         <v>0</v>
       </c>
       <c r="B22">
-        <v>0.7257599830627441</v>
+        <v>0.3002429008483887</v>
       </c>
       <c r="C22">
-        <v>0.01390886306762695</v>
+        <v>0.005982637405395508</v>
       </c>
       <c r="D22">
         <v>0.08615072104110666</v>
@@ -1344,10 +1344,10 @@
         <v>1</v>
       </c>
       <c r="B23">
-        <v>0.813230037689209</v>
+        <v>0.3130626678466797</v>
       </c>
       <c r="C23">
-        <v>0.006982326507568359</v>
+        <v>0.005982875823974609</v>
       </c>
       <c r="D23">
         <v>0.0810784054558117</v>
@@ -1385,10 +1385,10 @@
         <v>2</v>
       </c>
       <c r="B24">
-        <v>0.7748451232910156</v>
+        <v>0.3165256977081299</v>
       </c>
       <c r="C24">
-        <v>0.01595735549926758</v>
+        <v>0.004971981048583984</v>
       </c>
       <c r="D24">
         <v>0.08014337128532922</v>
@@ -1426,10 +1426,10 @@
         <v>3</v>
       </c>
       <c r="B25">
-        <v>0.7679753303527832</v>
+        <v>0.3273334503173828</v>
       </c>
       <c r="C25">
-        <v>0.008985757827758789</v>
+        <v>0.005983352661132812</v>
       </c>
       <c r="D25">
         <v>0.07714458539882736</v>
@@ -1467,10 +1467,10 @@
         <v>4</v>
       </c>
       <c r="B26">
-        <v>0.8211798667907715</v>
+        <v>0.3226416110992432</v>
       </c>
       <c r="C26">
-        <v>0.03289389610290527</v>
+        <v>0.005247831344604492</v>
       </c>
       <c r="D26">
         <v>0.07825350216121257</v>
@@ -1508,10 +1508,10 @@
         <v>0</v>
       </c>
       <c r="B27">
-        <v>3.590620756149292</v>
+        <v>0.8427574634552002</v>
       </c>
       <c r="C27">
-        <v>0.106208324432373</v>
+        <v>0.04801821708679199</v>
       </c>
       <c r="D27">
         <v>0.1016884406733621</v>
@@ -1549,10 +1549,10 @@
         <v>1</v>
       </c>
       <c r="B28">
-        <v>2.383957386016846</v>
+        <v>0.9223864078521729</v>
       </c>
       <c r="C28">
-        <v>0.08875060081481934</v>
+        <v>0.04850554466247559</v>
       </c>
       <c r="D28">
         <v>0.08896745158819719</v>
@@ -1590,10 +1590,10 @@
         <v>2</v>
       </c>
       <c r="B29">
-        <v>2.331623315811157</v>
+        <v>0.8076572418212891</v>
       </c>
       <c r="C29">
-        <v>0.09969472885131836</v>
+        <v>0.04718184471130371</v>
       </c>
       <c r="D29">
         <v>0.08519480198371109</v>
@@ -1631,10 +1631,10 @@
         <v>3</v>
       </c>
       <c r="B30">
-        <v>2.33028244972229</v>
+        <v>0.8806717395782471</v>
       </c>
       <c r="C30">
-        <v>0.1009864807128906</v>
+        <v>0.0488746166229248</v>
       </c>
       <c r="D30">
         <v>0.07915359220472561</v>
@@ -1672,10 +1672,10 @@
         <v>4</v>
       </c>
       <c r="B31">
-        <v>2.133999109268188</v>
+        <v>0.843618631362915</v>
       </c>
       <c r="C31">
-        <v>0.09800076484680176</v>
+        <v>0.04787135124206543</v>
       </c>
       <c r="D31">
         <v>0.0788070624137492</v>
@@ -1713,10 +1713,10 @@
         <v>0</v>
       </c>
       <c r="B32">
-        <v>3.164886236190796</v>
+        <v>2.938529491424561</v>
       </c>
       <c r="C32">
-        <v>0.02596521377563477</v>
+        <v>0.02655601501464844</v>
       </c>
       <c r="D32">
         <v>0.08226532370053968</v>
@@ -1754,10 +1754,10 @@
         <v>1</v>
       </c>
       <c r="B33">
-        <v>3.026375532150269</v>
+        <v>2.943948030471802</v>
       </c>
       <c r="C33">
-        <v>0.02593231201171875</v>
+        <v>0.02695322036743164</v>
       </c>
       <c r="D33">
         <v>0.08485306474010798</v>
@@ -1795,10 +1795,10 @@
         <v>2</v>
       </c>
       <c r="B34">
-        <v>3.234138011932373</v>
+        <v>3.116305828094482</v>
       </c>
       <c r="C34">
-        <v>0.02639937400817871</v>
+        <v>0.02593159675598145</v>
       </c>
       <c r="D34">
         <v>0.08215390790252361</v>
@@ -1836,10 +1836,10 @@
         <v>3</v>
       </c>
       <c r="B35">
-        <v>3.520739555358887</v>
+        <v>2.972084045410156</v>
       </c>
       <c r="C35">
-        <v>0.02910065650939941</v>
+        <v>0.024932861328125</v>
       </c>
       <c r="D35">
         <v>0.0768304974699239</v>
@@ -1877,10 +1877,10 @@
         <v>4</v>
       </c>
       <c r="B36">
-        <v>3.59433913230896</v>
+        <v>2.960963726043701</v>
       </c>
       <c r="C36">
-        <v>0.02663779258728027</v>
+        <v>0.02692818641662598</v>
       </c>
       <c r="D36">
         <v>0.07808364833618173</v>
@@ -1918,10 +1918,10 @@
         <v>0</v>
       </c>
       <c r="B37">
-        <v>0.4008901119232178</v>
+        <v>0.3869633674621582</v>
       </c>
       <c r="C37">
-        <v>0.004986763000488281</v>
+        <v>0.004987955093383789</v>
       </c>
       <c r="D37">
         <v>0.08245624737706117</v>
@@ -1959,10 +1959,10 @@
         <v>1</v>
       </c>
       <c r="B38">
-        <v>0.3959763050079346</v>
+        <v>0.3979356288909912</v>
       </c>
       <c r="C38">
-        <v>0.007325172424316406</v>
+        <v>0.005984783172607422</v>
       </c>
       <c r="D38">
         <v>0.08388607575828061</v>
@@ -2000,10 +2000,10 @@
         <v>2</v>
       </c>
       <c r="B39">
-        <v>0.4480743408203125</v>
+        <v>0.3901298046112061</v>
       </c>
       <c r="C39">
-        <v>0.005012035369873047</v>
+        <v>0.00600123405456543</v>
       </c>
       <c r="D39">
         <v>0.08451480144657204</v>
@@ -2041,10 +2041,10 @@
         <v>3</v>
       </c>
       <c r="B40">
-        <v>0.456615686416626</v>
+        <v>0.3948736190795898</v>
       </c>
       <c r="C40">
-        <v>0.00644993782043457</v>
+        <v>0.005010128021240234</v>
       </c>
       <c r="D40">
         <v>0.07857210659523567</v>
@@ -2082,10 +2082,10 @@
         <v>4</v>
       </c>
       <c r="B41">
-        <v>0.4879341125488281</v>
+        <v>0.3976535797119141</v>
       </c>
       <c r="C41">
-        <v>0.007978677749633789</v>
+        <v>0.005981922149658203</v>
       </c>
       <c r="D41">
         <v>0.08084260748252327</v>
@@ -2123,10 +2123,10 @@
         <v>0</v>
       </c>
       <c r="B42">
-        <v>1.014837026596069</v>
+        <v>0.895395040512085</v>
       </c>
       <c r="C42">
-        <v>0.0459752082824707</v>
+        <v>0.04595398902893066</v>
       </c>
       <c r="D42">
         <v>0.09523434305141333</v>
@@ -2164,10 +2164,10 @@
         <v>1</v>
       </c>
       <c r="B43">
-        <v>1.013093948364258</v>
+        <v>0.8732194900512695</v>
       </c>
       <c r="C43">
-        <v>0.04729986190795898</v>
+        <v>0.04443144798278809</v>
       </c>
       <c r="D43">
         <v>0.08852478258833088</v>
@@ -2205,10 +2205,10 @@
         <v>2</v>
       </c>
       <c r="B44">
-        <v>0.9654896259307861</v>
+        <v>0.8133976459503174</v>
       </c>
       <c r="C44">
-        <v>0.04515647888183594</v>
+        <v>0.0438995361328125</v>
       </c>
       <c r="D44">
         <v>0.08732828147159429</v>
@@ -2246,10 +2246,10 @@
         <v>3</v>
       </c>
       <c r="B45">
-        <v>1.333621978759766</v>
+        <v>0.8989794254302979</v>
       </c>
       <c r="C45">
-        <v>0.05585312843322754</v>
+        <v>0.04589366912841797</v>
       </c>
       <c r="D45">
         <v>0.07899686196740759</v>
@@ -2287,10 +2287,10 @@
         <v>4</v>
       </c>
       <c r="B46">
-        <v>1.080972671508789</v>
+        <v>0.8760039806365967</v>
       </c>
       <c r="C46">
-        <v>0.05130243301391602</v>
+        <v>0.04485082626342773</v>
       </c>
       <c r="D46">
         <v>0.0837282957808414</v>
@@ -2328,10 +2328,10 @@
         <v>0</v>
       </c>
       <c r="B47">
-        <v>9.198221206665039</v>
+        <v>3.658556938171387</v>
       </c>
       <c r="C47">
-        <v>0.1326522827148438</v>
+        <v>0.02590513229370117</v>
       </c>
       <c r="D47">
         <v>0.08610622733158727</v>
@@ -2369,10 +2369,10 @@
         <v>1</v>
       </c>
       <c r="B48">
-        <v>6.843193054199219</v>
+        <v>3.548771858215332</v>
       </c>
       <c r="C48">
-        <v>0.06980085372924805</v>
+        <v>0.0269775390625</v>
       </c>
       <c r="D48">
         <v>0.08421381989488307</v>
@@ -2410,10 +2410,10 @@
         <v>2</v>
       </c>
       <c r="B49">
-        <v>7.524701595306396</v>
+        <v>3.643791198730469</v>
       </c>
       <c r="C49">
-        <v>0.08015298843383789</v>
+        <v>0.0259251594543457</v>
       </c>
       <c r="D49">
         <v>0.08228061663942059</v>
@@ -2451,10 +2451,10 @@
         <v>3</v>
       </c>
       <c r="B50">
-        <v>6.883135557174683</v>
+        <v>3.587129831314087</v>
       </c>
       <c r="C50">
-        <v>0.03693485260009766</v>
+        <v>0.02589941024780273</v>
       </c>
       <c r="D50">
         <v>0.07855459770114939</v>
@@ -2492,10 +2492,10 @@
         <v>4</v>
       </c>
       <c r="B51">
-        <v>6.922020673751831</v>
+        <v>3.58620023727417</v>
       </c>
       <c r="C51">
-        <v>0.06284832954406738</v>
+        <v>0.04695987701416016</v>
       </c>
       <c r="D51">
         <v>0.07736269939010079</v>
@@ -2533,10 +2533,10 @@
         <v>0</v>
       </c>
       <c r="B52">
-        <v>1.43100905418396</v>
+        <v>0.7154374122619629</v>
       </c>
       <c r="C52">
-        <v>0.03988504409790039</v>
+        <v>0.006982326507568359</v>
       </c>
       <c r="D52">
         <v>0.09245643247349206</v>
@@ -2574,10 +2574,10 @@
         <v>1</v>
       </c>
       <c r="B53">
-        <v>3.51714563369751</v>
+        <v>0.7470018863677979</v>
       </c>
       <c r="C53">
-        <v>0.01895260810852051</v>
+        <v>0.005990505218505859</v>
       </c>
       <c r="D53">
         <v>0.08245001384328449</v>
@@ -2615,10 +2615,10 @@
         <v>2</v>
       </c>
       <c r="B54">
-        <v>1.412550210952759</v>
+        <v>0.5455429553985596</v>
       </c>
       <c r="C54">
-        <v>0.02786731719970703</v>
+        <v>0.005982637405395508</v>
       </c>
       <c r="D54">
         <v>0.08404507727171119</v>
@@ -2656,10 +2656,10 @@
         <v>3</v>
       </c>
       <c r="B55">
-        <v>1.435384273529053</v>
+        <v>0.6482686996459961</v>
       </c>
       <c r="C55">
-        <v>0.0131528377532959</v>
+        <v>0.005982875823974609</v>
       </c>
       <c r="D55">
         <v>0.08388427639829701</v>
@@ -2697,10 +2697,10 @@
         <v>4</v>
       </c>
       <c r="B56">
-        <v>1.803934574127197</v>
+        <v>0.6023893356323242</v>
       </c>
       <c r="C56">
-        <v>0.02240109443664551</v>
+        <v>0.005984067916870117</v>
       </c>
       <c r="D56">
         <v>0.08108824353499955</v>
@@ -2738,10 +2738,10 @@
         <v>0</v>
       </c>
       <c r="B57">
-        <v>5.378308057785034</v>
+        <v>1.627213001251221</v>
       </c>
       <c r="C57">
-        <v>0.1152057647705078</v>
+        <v>0.04787087440490723</v>
       </c>
       <c r="D57">
         <v>0.09650335461024566</v>
@@ -2779,10 +2779,10 @@
         <v>1</v>
       </c>
       <c r="B58">
-        <v>5.221487998962402</v>
+        <v>1.524784564971924</v>
       </c>
       <c r="C58">
-        <v>0.1283807754516602</v>
+        <v>0.04690146446228027</v>
       </c>
       <c r="D58">
         <v>0.09141827634489097</v>
@@ -2820,10 +2820,10 @@
         <v>2</v>
       </c>
       <c r="B59">
-        <v>5.107499361038208</v>
+        <v>1.517983436584473</v>
       </c>
       <c r="C59">
-        <v>0.1159701347351074</v>
+        <v>0.04886889457702637</v>
       </c>
       <c r="D59">
         <v>0.08782892788648006</v>
@@ -2861,10 +2861,10 @@
         <v>3</v>
       </c>
       <c r="B60">
-        <v>4.725463151931763</v>
+        <v>1.811950445175171</v>
       </c>
       <c r="C60">
-        <v>0.1146910190582275</v>
+        <v>0.05089426040649414</v>
       </c>
       <c r="D60">
         <v>0.08341557341928783</v>
@@ -2902,10 +2902,10 @@
         <v>4</v>
       </c>
       <c r="B61">
-        <v>4.269973039627075</v>
+        <v>1.524324178695679</v>
       </c>
       <c r="C61">
-        <v>0.1031033992767334</v>
+        <v>0.04997515678405762</v>
       </c>
       <c r="D61">
         <v>0.08102874558971447</v>

</xml_diff>